<commit_message>
refactoring some code. pushing new result file
</commit_message>
<xml_diff>
--- a/output/predix-catalog.xlsx
+++ b/output/predix-catalog.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="503">
   <si>
     <t># Available Categories</t>
   </si>
@@ -23,7 +23,7 @@
     <t># Available Services</t>
   </si>
   <si>
-    <t>File generated on:2016/11/04 18:53:30</t>
+    <t>File generated on:2016/11/06 14:11:45</t>
   </si>
   <si>
     <t>Using 'predix-catalog-scraper' - https://github.com/indaco/predix-catalog-scraper</t>
@@ -132,6 +132,34 @@
   </si>
   <si>
     <t xml:space="preserve"> 05/11/16
+</t>
+  </si>
+  <si>
+    <t>Enterprise Connect</t>
+  </si>
+  <si>
+    <t>Predix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide manageable and scalable connectivity between the Predix cloud and your enterprise. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This service uses Websockets to securely support all TCP protocols for scalable and flexible deployment. 
+Enterprise Connect also provides:
+Connection of enterprise resources from Predix to on-premises resources
+ETL capability between the cloud and on-premises resources using existing software for integration
+Enterprise proxy service friendly
+Integrated authentication and authorization using UAA with OAUTH 
+Reach-back between the cloud and on-premises over WSS protocol
+Native protocol access to on-premises resources over standard ports like WS, JDBC, File access, FTP, etc.
+Scalable and lightweight solutions
+</t>
+  </si>
+  <si>
+    <t>https://www.predix.io/services/service.html?id=2184</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/04/16
 </t>
   </si>
   <si>
@@ -397,6 +425,28 @@
     <t>https://www.predix.io/services/service.html?id=1182</t>
   </si>
   <si>
+    <t>Unit of Measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use this service to convert one measurement unit to another (in beta). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit of Measure (in beta) is a full-fledged engineering unit-of-measure conversion module with batch conversion capability, configurability across single/group units, and streaming conversion in near or real time.
+The service supports ingestion of time-series data into Predix as well as consumption of the visualization and analytics engine from the Predix Time Series service.
+Key features include:
+Set up the configurations for all the expressions in the standard library
+Use the conversion service to do the unit conversion from one unit to the other
+Apply the batch conversion capability using json or CSV input
+Use tenant-based custom configuration and conversion facility
+Electric submersible pumps (ESP’s) using surface and subsurface sensors capture equipment and well-bore condition data in various units of measure depending on the location of the wells.
+Oil Field Analytics products used at the Well sites typically transmit the aggregated data in batches for persistence; the raw data units in the batch are converted into standard units (si) of data before the data are persisted in the Time Series database.
+Streaming data from the Remote Terminal Units (RTU’s) collecting data on the well sites is converted on-the-fly to standard units before the data are persisted in the Time series database.
+</t>
+  </si>
+  <si>
+    <t>https://www.predix.io/services/service.html?id=2185</t>
+  </si>
+  <si>
     <t>Key-Value Store</t>
   </si>
   <si>
@@ -514,9 +564,6 @@
   </si>
   <si>
     <t>Analytics Framework</t>
-  </si>
-  <si>
-    <t>Predix</t>
   </si>
   <si>
     <t xml:space="preserve">Deploy, orchestrate, and schedule analytics to execute in Predix, and upload your own, or add analytics from the Analytics tab.
@@ -1279,6 +1326,9 @@
   </si>
   <si>
     <t>https://www.predix.io/services/service.html?id=1231</t>
+  </si>
+  <si>
+    <t>File generated on:2016/11/06 14:12:12</t>
   </si>
   <si>
     <t>Trend Anomaly Detection</t>
@@ -2418,23 +2468,6 @@
     <t>https://www.predix.io/analytics/analytic.html?id=1944</t>
   </si>
   <si>
-    <t>Cluster Analysis</t>
-  </si>
-  <si>
-    <t>This unsupervised method organizes similar objects into specific clusters.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-This service organizes objects in the same cluster that are more similar to each other than to those objects in other clusters.
-Either of two methods can be applied to perform the clustering:
-Agglomerative Clustering builds a hierarchy of clusters. "Ward" linkage has been implemented in this microservice.
-K-means is a simple, unsupervised learning algorithm to solve a clustering problem. The procedure classifies a given dataset through a specific number of clusters (assume K clusters) fixed apriori.
-</t>
-  </si>
-  <si>
-    <t>https://www.predix.io/analytics/analytic.html?id=1942</t>
-  </si>
-  <si>
     <t>Density Based Spatial Clustering</t>
   </si>
   <si>
@@ -2453,6 +2486,23 @@
   </si>
   <si>
     <t>https://www.predix.io/analytics/analytic.html?id=2079</t>
+  </si>
+  <si>
+    <t>Cluster Analysis</t>
+  </si>
+  <si>
+    <t>This unsupervised method organizes similar objects into specific clusters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+This service organizes objects in the same cluster that are more similar to each other than to those objects in other clusters.
+Either of two methods can be applied to perform the clustering:
+Agglomerative Clustering builds a hierarchy of clusters. "Ward" linkage has been implemented in this microservice.
+K-means is a simple, unsupervised learning algorithm to solve a clustering problem. The procedure classifies a given dataset through a specific number of clusters (assume K clusters) fixed apriori.
+</t>
+  </si>
+  <si>
+    <t>https://www.predix.io/analytics/analytic.html?id=1942</t>
   </si>
   <si>
     <t>Energy Price Prediction - Training Model</t>
@@ -2834,7 +2884,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2866,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -2958,30 +3008,30 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
@@ -2999,15 +3049,15 @@
         <v>35</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
@@ -3016,24 +3066,24 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
@@ -3042,30 +3092,30 @@
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>48</v>
@@ -3077,189 +3127,189 @@
         <v>50</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="H16" s="2" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="H17" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>78</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3267,7 +3317,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
@@ -3285,7 +3335,7 @@
         <v>90</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3293,33 +3343,33 @@
         <v>91</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
@@ -3328,50 +3378,50 @@
         <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="H22" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
@@ -3380,30 +3430,30 @@
         <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>113</v>
@@ -3415,21 +3465,21 @@
         <v>115</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>45</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>118</v>
@@ -3441,59 +3491,59 @@
         <v>120</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>121</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="H27" s="2" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -3501,65 +3551,65 @@
         <v>131</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="H30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>143</v>
@@ -3571,221 +3621,221 @@
         <v>145</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="G38" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="G39" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="H39" s="2" t="s">
-        <v>186</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>21</v>
@@ -3794,42 +3844,42 @@
         <v>15</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3837,7 +3887,7 @@
         <v>196</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>21</v>
@@ -3855,7 +3905,7 @@
         <v>199</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>180</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3863,103 +3913,155 @@
         <v>200</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="H43" s="2" t="s">
-        <v>206</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>211</v>
-      </c>
       <c r="H44" s="2" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="G45" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="G46" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>164</v>
+      <c r="B47" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4005,6 +4107,8 @@
     <hyperlink ref="G44" r:id="rId39"/>
     <hyperlink ref="G45" r:id="rId40"/>
     <hyperlink ref="G46" r:id="rId41"/>
+    <hyperlink ref="G47" r:id="rId42"/>
+    <hyperlink ref="G48" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4036,7 +4140,7 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4078,1640 +4182,1640 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>462</v>
+        <v>472</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>463</v>
+        <v>473</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
-        <v>464</v>
+        <v>474</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E62" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>468</v>
+        <v>478</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>471</v>
+        <v>481</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>472</v>
+        <v>482</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="2" t="s">
-        <v>473</v>
+        <v>483</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="2" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>478</v>
+        <v>488</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>479</v>
+        <v>489</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="2" t="s">
-        <v>481</v>
+        <v>491</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>482</v>
+        <v>492</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>483</v>
+        <v>493</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>484</v>
+        <v>494</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
-        <v>485</v>
+        <v>495</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>486</v>
+        <v>496</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="2" t="s">
-        <v>489</v>
+        <v>499</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>469</v>
+        <v>479</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>491</v>
+        <v>501</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>492</v>
+        <v>502</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>